<commit_message>
Correct hierarchical split, compare distance matrices, precompute, calculate informations on divisive, observe divisive construction
</commit_message>
<xml_diff>
--- a/Code/data/first_axis_labels.xlsx
+++ b/Code/data/first_axis_labels.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>distance axe début m</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Ref_label</t>
+  </si>
+  <si>
+    <t>Divi_label_Th0.9</t>
   </si>
 </sst>
 </file>
@@ -440,13 +443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W196"/>
+  <dimension ref="A1:X196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,8 +519,11 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>0</v>
       </c>
@@ -587,8 +593,11 @@
       <c r="W2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>50</v>
       </c>
@@ -658,8 +667,11 @@
       <c r="W3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="X3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>100</v>
       </c>
@@ -729,8 +741,11 @@
       <c r="W4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="X4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>150</v>
       </c>
@@ -800,8 +815,11 @@
       <c r="W5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="X5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>200</v>
       </c>
@@ -871,8 +889,11 @@
       <c r="W6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="X6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>394.929</v>
       </c>
@@ -942,8 +963,11 @@
       <c r="W7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="X7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>450</v>
       </c>
@@ -1013,8 +1037,11 @@
       <c r="W8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="X8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>500</v>
       </c>
@@ -1084,8 +1111,11 @@
       <c r="W9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="X9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>550</v>
       </c>
@@ -1155,8 +1185,11 @@
       <c r="W10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="X10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11">
         <v>600</v>
       </c>
@@ -1226,8 +1259,11 @@
       <c r="W11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="X11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12">
         <v>650</v>
       </c>
@@ -1297,8 +1333,11 @@
       <c r="W12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="X12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13">
         <v>700</v>
       </c>
@@ -1368,8 +1407,11 @@
       <c r="W13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="X13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>750</v>
       </c>
@@ -1439,8 +1481,11 @@
       <c r="W14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="X14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15">
         <v>800</v>
       </c>
@@ -1510,8 +1555,11 @@
       <c r="W15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="X15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16">
         <v>850</v>
       </c>
@@ -1581,8 +1629,11 @@
       <c r="W16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="X16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>900</v>
       </c>
@@ -1652,8 +1703,11 @@
       <c r="W17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="X17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18">
         <v>950</v>
       </c>
@@ -1723,8 +1777,11 @@
       <c r="W18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="X18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19">
         <v>1000</v>
       </c>
@@ -1794,8 +1851,11 @@
       <c r="W19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="X19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20">
         <v>1050</v>
       </c>
@@ -1865,8 +1925,11 @@
       <c r="W20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="X20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21">
         <v>1100</v>
       </c>
@@ -1936,8 +1999,11 @@
       <c r="W21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="X21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>1150</v>
       </c>
@@ -2007,8 +2073,11 @@
       <c r="W22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="X22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>1200</v>
       </c>
@@ -2078,8 +2147,11 @@
       <c r="W23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="X23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>1250</v>
       </c>
@@ -2149,8 +2221,11 @@
       <c r="W24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="X24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>1300</v>
       </c>
@@ -2220,8 +2295,11 @@
       <c r="W25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="X25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>1350</v>
       </c>
@@ -2291,8 +2369,11 @@
       <c r="W26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="X26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>1400</v>
       </c>
@@ -2362,8 +2443,11 @@
       <c r="W27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:23">
+      <c r="X27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28">
         <v>1450</v>
       </c>
@@ -2433,8 +2517,11 @@
       <c r="W28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="X28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29">
         <v>1500</v>
       </c>
@@ -2504,8 +2591,11 @@
       <c r="W29">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:23">
+      <c r="X29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30">
         <v>1550</v>
       </c>
@@ -2575,8 +2665,11 @@
       <c r="W30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:23">
+      <c r="X30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31">
         <v>1600</v>
       </c>
@@ -2646,8 +2739,11 @@
       <c r="W31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:23">
+      <c r="X31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32">
         <v>1650</v>
       </c>
@@ -2717,8 +2813,11 @@
       <c r="W32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:23">
+      <c r="X32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33">
         <v>1700</v>
       </c>
@@ -2788,8 +2887,11 @@
       <c r="W33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:23">
+      <c r="X33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34">
         <v>1750</v>
       </c>
@@ -2859,8 +2961,11 @@
       <c r="W34">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:23">
+      <c r="X34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35">
         <v>1800</v>
       </c>
@@ -2930,8 +3035,11 @@
       <c r="W35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:23">
+      <c r="X35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36">
         <v>1850</v>
       </c>
@@ -3001,8 +3109,11 @@
       <c r="W36">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:23">
+      <c r="X36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
       <c r="A37">
         <v>1900</v>
       </c>
@@ -3072,8 +3183,11 @@
       <c r="W37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:23">
+      <c r="X37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
       <c r="A38">
         <v>1950</v>
       </c>
@@ -3143,8 +3257,11 @@
       <c r="W38">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:23">
+      <c r="X38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24">
       <c r="A39">
         <v>2000</v>
       </c>
@@ -3214,8 +3331,11 @@
       <c r="W39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:23">
+      <c r="X39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24">
       <c r="A40">
         <v>2050</v>
       </c>
@@ -3285,8 +3405,11 @@
       <c r="W40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:23">
+      <c r="X40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
       <c r="A41">
         <v>2100</v>
       </c>
@@ -3356,8 +3479,11 @@
       <c r="W41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:23">
+      <c r="X41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24">
       <c r="A42">
         <v>2150</v>
       </c>
@@ -3427,8 +3553,11 @@
       <c r="W42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:23">
+      <c r="X42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
       <c r="A43">
         <v>2200</v>
       </c>
@@ -3498,8 +3627,11 @@
       <c r="W43">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:23">
+      <c r="X43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24">
       <c r="A44">
         <v>2250</v>
       </c>
@@ -3569,8 +3701,11 @@
       <c r="W44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:23">
+      <c r="X44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24">
       <c r="A45">
         <v>2300</v>
       </c>
@@ -3640,8 +3775,11 @@
       <c r="W45">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:23">
+      <c r="X45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24">
       <c r="A46">
         <v>2350</v>
       </c>
@@ -3711,8 +3849,11 @@
       <c r="W46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:23">
+      <c r="X46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24">
       <c r="A47">
         <v>2400</v>
       </c>
@@ -3782,8 +3923,11 @@
       <c r="W47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:23">
+      <c r="X47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
       <c r="A48">
         <v>2450</v>
       </c>
@@ -3853,8 +3997,11 @@
       <c r="W48">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:23">
+      <c r="X48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
       <c r="A49">
         <v>2500</v>
       </c>
@@ -3924,8 +4071,11 @@
       <c r="W49">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:23">
+      <c r="X49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
       <c r="A50">
         <v>2550</v>
       </c>
@@ -3995,8 +4145,11 @@
       <c r="W50">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:23">
+      <c r="X50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24">
       <c r="A51">
         <v>2600</v>
       </c>
@@ -4066,8 +4219,11 @@
       <c r="W51">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:23">
+      <c r="X51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
       <c r="A52">
         <v>2650</v>
       </c>
@@ -4137,8 +4293,11 @@
       <c r="W52">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:23">
+      <c r="X52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24">
       <c r="A53">
         <v>2700</v>
       </c>
@@ -4208,8 +4367,11 @@
       <c r="W53">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:23">
+      <c r="X53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24">
       <c r="A54">
         <v>2750</v>
       </c>
@@ -4279,8 +4441,11 @@
       <c r="W54">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:23">
+      <c r="X54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24">
       <c r="A55">
         <v>2800</v>
       </c>
@@ -4350,8 +4515,11 @@
       <c r="W55">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:23">
+      <c r="X55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24">
       <c r="A56">
         <v>2850</v>
       </c>
@@ -4421,8 +4589,11 @@
       <c r="W56">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:23">
+      <c r="X56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24">
       <c r="A57">
         <v>2900</v>
       </c>
@@ -4492,8 +4663,11 @@
       <c r="W57">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:23">
+      <c r="X57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24">
       <c r="A58">
         <v>2950</v>
       </c>
@@ -4563,8 +4737,11 @@
       <c r="W58">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:23">
+      <c r="X58">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24">
       <c r="A59">
         <v>3000</v>
       </c>
@@ -4634,8 +4811,11 @@
       <c r="W59">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:23">
+      <c r="X59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24">
       <c r="A60">
         <v>3050</v>
       </c>
@@ -4705,8 +4885,11 @@
       <c r="W60">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:23">
+      <c r="X60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24">
       <c r="A61">
         <v>3100</v>
       </c>
@@ -4776,8 +4959,11 @@
       <c r="W61">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:23">
+      <c r="X61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24">
       <c r="A62">
         <v>3150</v>
       </c>
@@ -4847,8 +5033,11 @@
       <c r="W62">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:23">
+      <c r="X62">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24">
       <c r="A63">
         <v>3200</v>
       </c>
@@ -4918,8 +5107,11 @@
       <c r="W63">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:23">
+      <c r="X63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24">
       <c r="A64">
         <v>3250</v>
       </c>
@@ -4989,8 +5181,11 @@
       <c r="W64">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:23">
+      <c r="X64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24">
       <c r="A65">
         <v>3300</v>
       </c>
@@ -5060,8 +5255,11 @@
       <c r="W65">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:23">
+      <c r="X65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24">
       <c r="A66">
         <v>3350</v>
       </c>
@@ -5131,8 +5329,11 @@
       <c r="W66">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:23">
+      <c r="X66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24">
       <c r="A67">
         <v>3400</v>
       </c>
@@ -5202,8 +5403,11 @@
       <c r="W67">
         <v>7</v>
       </c>
-    </row>
-    <row r="68" spans="1:23">
+      <c r="X67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24">
       <c r="A68">
         <v>3450</v>
       </c>
@@ -5273,8 +5477,11 @@
       <c r="W68">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:23">
+      <c r="X68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24">
       <c r="A69">
         <v>3500</v>
       </c>
@@ -5344,8 +5551,11 @@
       <c r="W69">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:23">
+      <c r="X69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24">
       <c r="A70">
         <v>3550</v>
       </c>
@@ -5415,8 +5625,11 @@
       <c r="W70">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:23">
+      <c r="X70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24">
       <c r="A71">
         <v>3600</v>
       </c>
@@ -5486,8 +5699,11 @@
       <c r="W71">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:23">
+      <c r="X71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24">
       <c r="A72">
         <v>3650</v>
       </c>
@@ -5557,8 +5773,11 @@
       <c r="W72">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:23">
+      <c r="X72">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24">
       <c r="A73">
         <v>3700</v>
       </c>
@@ -5628,8 +5847,11 @@
       <c r="W73">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:23">
+      <c r="X73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24">
       <c r="A74">
         <v>3750</v>
       </c>
@@ -5699,8 +5921,11 @@
       <c r="W74">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:23">
+      <c r="X74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24">
       <c r="A75">
         <v>3800</v>
       </c>
@@ -5770,8 +5995,11 @@
       <c r="W75">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:23">
+      <c r="X75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24">
       <c r="A76">
         <v>3850</v>
       </c>
@@ -5841,8 +6069,11 @@
       <c r="W76">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:23">
+      <c r="X76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24">
       <c r="A77">
         <v>3900</v>
       </c>
@@ -5912,8 +6143,11 @@
       <c r="W77">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:23">
+      <c r="X77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24">
       <c r="A78">
         <v>3950</v>
       </c>
@@ -5983,8 +6217,11 @@
       <c r="W78">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:23">
+      <c r="X78">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24">
       <c r="A79">
         <v>4000</v>
       </c>
@@ -6054,8 +6291,11 @@
       <c r="W79">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:23">
+      <c r="X79">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24">
       <c r="A80">
         <v>4050</v>
       </c>
@@ -6125,8 +6365,11 @@
       <c r="W80">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:23">
+      <c r="X80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24">
       <c r="A81">
         <v>4100</v>
       </c>
@@ -6196,8 +6439,11 @@
       <c r="W81">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:23">
+      <c r="X81">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24">
       <c r="A82">
         <v>4150</v>
       </c>
@@ -6267,8 +6513,11 @@
       <c r="W82">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:23">
+      <c r="X82">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24">
       <c r="A83">
         <v>4200</v>
       </c>
@@ -6338,8 +6587,11 @@
       <c r="W83">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:23">
+      <c r="X83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24">
       <c r="A84">
         <v>4250</v>
       </c>
@@ -6409,8 +6661,11 @@
       <c r="W84">
         <v>8</v>
       </c>
-    </row>
-    <row r="85" spans="1:23">
+      <c r="X84">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24">
       <c r="A85">
         <v>4300</v>
       </c>
@@ -6480,8 +6735,11 @@
       <c r="W85">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:23">
+      <c r="X85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24">
       <c r="A86">
         <v>4350</v>
       </c>
@@ -6551,8 +6809,11 @@
       <c r="W86">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="1:23">
+      <c r="X86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24">
       <c r="A87">
         <v>4400</v>
       </c>
@@ -6622,8 +6883,11 @@
       <c r="W87">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="1:23">
+      <c r="X87">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24">
       <c r="A88">
         <v>4450</v>
       </c>
@@ -6693,8 +6957,11 @@
       <c r="W88">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="1:23">
+      <c r="X88">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24">
       <c r="A89">
         <v>4500</v>
       </c>
@@ -6764,8 +7031,11 @@
       <c r="W89">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:23">
+      <c r="X89">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24">
       <c r="A90">
         <v>4550</v>
       </c>
@@ -6835,8 +7105,11 @@
       <c r="W90">
         <v>8</v>
       </c>
-    </row>
-    <row r="91" spans="1:23">
+      <c r="X90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24">
       <c r="A91">
         <v>4600</v>
       </c>
@@ -6906,8 +7179,11 @@
       <c r="W91">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:23">
+      <c r="X91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24">
       <c r="A92">
         <v>4650</v>
       </c>
@@ -6977,8 +7253,11 @@
       <c r="W92">
         <v>8</v>
       </c>
-    </row>
-    <row r="93" spans="1:23">
+      <c r="X92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24">
       <c r="A93">
         <v>4700</v>
       </c>
@@ -7048,8 +7327,11 @@
       <c r="W93">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:23">
+      <c r="X93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24">
       <c r="A94">
         <v>4750</v>
       </c>
@@ -7119,8 +7401,11 @@
       <c r="W94">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="1:23">
+      <c r="X94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24">
       <c r="A95">
         <v>4800</v>
       </c>
@@ -7190,8 +7475,11 @@
       <c r="W95">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:23">
+      <c r="X95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24">
       <c r="A96">
         <v>4850</v>
       </c>
@@ -7261,8 +7549,11 @@
       <c r="W96">
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="1:23">
+      <c r="X96">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24">
       <c r="A97">
         <v>4900</v>
       </c>
@@ -7332,8 +7623,11 @@
       <c r="W97">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:23">
+      <c r="X97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24">
       <c r="A98">
         <v>4950</v>
       </c>
@@ -7403,8 +7697,11 @@
       <c r="W98">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:23">
+      <c r="X98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24">
       <c r="A99">
         <v>5000</v>
       </c>
@@ -7474,8 +7771,11 @@
       <c r="W99">
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="1:23">
+      <c r="X99">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24">
       <c r="A100">
         <v>5050</v>
       </c>
@@ -7545,8 +7845,11 @@
       <c r="W100">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:23">
+      <c r="X100">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24">
       <c r="A101">
         <v>5100</v>
       </c>
@@ -7616,8 +7919,11 @@
       <c r="W101">
         <v>8</v>
       </c>
-    </row>
-    <row r="102" spans="1:23">
+      <c r="X101">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24">
       <c r="A102">
         <v>5150</v>
       </c>
@@ -7687,8 +7993,11 @@
       <c r="W102">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:23">
+      <c r="X102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24">
       <c r="A103">
         <v>5200</v>
       </c>
@@ -7758,8 +8067,11 @@
       <c r="W103">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:23">
+      <c r="X103">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24">
       <c r="A104">
         <v>5250</v>
       </c>
@@ -7829,8 +8141,11 @@
       <c r="W104">
         <v>8</v>
       </c>
-    </row>
-    <row r="105" spans="1:23">
+      <c r="X104">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24">
       <c r="A105">
         <v>5300</v>
       </c>
@@ -7900,8 +8215,11 @@
       <c r="W105">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:23">
+      <c r="X105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24">
       <c r="A106">
         <v>5350</v>
       </c>
@@ -7971,8 +8289,11 @@
       <c r="W106">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:23">
+      <c r="X106">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24">
       <c r="A107">
         <v>5400</v>
       </c>
@@ -8042,8 +8363,11 @@
       <c r="W107">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:23">
+      <c r="X107">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24">
       <c r="A108">
         <v>5450</v>
       </c>
@@ -8113,8 +8437,11 @@
       <c r="W108">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="1:23">
+      <c r="X108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24">
       <c r="A109">
         <v>5500</v>
       </c>
@@ -8184,8 +8511,11 @@
       <c r="W109">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:23">
+      <c r="X109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24">
       <c r="A110">
         <v>5550</v>
       </c>
@@ -8255,8 +8585,11 @@
       <c r="W110">
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:23">
+      <c r="X110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24">
       <c r="A111">
         <v>5600</v>
       </c>
@@ -8326,8 +8659,11 @@
       <c r="W111">
         <v>8</v>
       </c>
-    </row>
-    <row r="112" spans="1:23">
+      <c r="X111">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24">
       <c r="A112">
         <v>5650</v>
       </c>
@@ -8397,8 +8733,11 @@
       <c r="W112">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:23">
+      <c r="X112">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24">
       <c r="A113">
         <v>5700</v>
       </c>
@@ -8468,8 +8807,11 @@
       <c r="W113">
         <v>8</v>
       </c>
-    </row>
-    <row r="114" spans="1:23">
+      <c r="X113">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24">
       <c r="A114">
         <v>5750</v>
       </c>
@@ -8539,8 +8881,11 @@
       <c r="W114">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="1:23">
+      <c r="X114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24">
       <c r="A115">
         <v>5800</v>
       </c>
@@ -8610,8 +8955,11 @@
       <c r="W115">
         <v>8</v>
       </c>
-    </row>
-    <row r="116" spans="1:23">
+      <c r="X115">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24">
       <c r="A116">
         <v>5850</v>
       </c>
@@ -8681,8 +9029,11 @@
       <c r="W116">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="1:23">
+      <c r="X116">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24">
       <c r="A117">
         <v>5900</v>
       </c>
@@ -8752,8 +9103,11 @@
       <c r="W117">
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:23">
+      <c r="X117">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24">
       <c r="A118">
         <v>5950</v>
       </c>
@@ -8823,8 +9177,11 @@
       <c r="W118">
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:23">
+      <c r="X118">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24">
       <c r="A119">
         <v>6000</v>
       </c>
@@ -8894,8 +9251,11 @@
       <c r="W119">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:23">
+      <c r="X119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24">
       <c r="A120">
         <v>6050</v>
       </c>
@@ -8965,8 +9325,11 @@
       <c r="W120">
         <v>8</v>
       </c>
-    </row>
-    <row r="121" spans="1:23">
+      <c r="X120">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24">
       <c r="A121">
         <v>6100</v>
       </c>
@@ -9036,8 +9399,11 @@
       <c r="W121">
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:23">
+      <c r="X121">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24">
       <c r="A122">
         <v>6150</v>
       </c>
@@ -9107,8 +9473,11 @@
       <c r="W122">
         <v>8</v>
       </c>
-    </row>
-    <row r="123" spans="1:23">
+      <c r="X122">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24">
       <c r="A123">
         <v>6200</v>
       </c>
@@ -9178,8 +9547,11 @@
       <c r="W123">
         <v>8</v>
       </c>
-    </row>
-    <row r="124" spans="1:23">
+      <c r="X123">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24">
       <c r="A124">
         <v>6250</v>
       </c>
@@ -9249,8 +9621,11 @@
       <c r="W124">
         <v>8</v>
       </c>
-    </row>
-    <row r="125" spans="1:23">
+      <c r="X124">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24">
       <c r="A125">
         <v>6300</v>
       </c>
@@ -9320,8 +9695,11 @@
       <c r="W125">
         <v>8</v>
       </c>
-    </row>
-    <row r="126" spans="1:23">
+      <c r="X125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24">
       <c r="A126">
         <v>6350</v>
       </c>
@@ -9391,8 +9769,11 @@
       <c r="W126">
         <v>10</v>
       </c>
-    </row>
-    <row r="127" spans="1:23">
+      <c r="X126">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:24">
       <c r="A127">
         <v>6400</v>
       </c>
@@ -9462,8 +9843,11 @@
       <c r="W127">
         <v>10</v>
       </c>
-    </row>
-    <row r="128" spans="1:23">
+      <c r="X127">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24">
       <c r="A128">
         <v>6450</v>
       </c>
@@ -9533,8 +9917,11 @@
       <c r="W128">
         <v>10</v>
       </c>
-    </row>
-    <row r="129" spans="1:23">
+      <c r="X128">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24">
       <c r="A129">
         <v>6500</v>
       </c>
@@ -9604,8 +9991,11 @@
       <c r="W129">
         <v>10</v>
       </c>
-    </row>
-    <row r="130" spans="1:23">
+      <c r="X129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24">
       <c r="A130">
         <v>6550</v>
       </c>
@@ -9675,8 +10065,11 @@
       <c r="W130">
         <v>10</v>
       </c>
-    </row>
-    <row r="131" spans="1:23">
+      <c r="X130">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24">
       <c r="A131">
         <v>6600</v>
       </c>
@@ -9746,8 +10139,11 @@
       <c r="W131">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:23">
+      <c r="X131">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24">
       <c r="A132">
         <v>6650</v>
       </c>
@@ -9817,8 +10213,11 @@
       <c r="W132">
         <v>10</v>
       </c>
-    </row>
-    <row r="133" spans="1:23">
+      <c r="X132">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24">
       <c r="A133">
         <v>6700</v>
       </c>
@@ -9888,8 +10287,11 @@
       <c r="W133">
         <v>10</v>
       </c>
-    </row>
-    <row r="134" spans="1:23">
+      <c r="X133">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24">
       <c r="A134">
         <v>6750</v>
       </c>
@@ -9959,8 +10361,11 @@
       <c r="W134">
         <v>10</v>
       </c>
-    </row>
-    <row r="135" spans="1:23">
+      <c r="X134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24">
       <c r="A135">
         <v>6800</v>
       </c>
@@ -10030,8 +10435,11 @@
       <c r="W135">
         <v>10</v>
       </c>
-    </row>
-    <row r="136" spans="1:23">
+      <c r="X135">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24">
       <c r="A136">
         <v>6850</v>
       </c>
@@ -10101,8 +10509,11 @@
       <c r="W136">
         <v>10</v>
       </c>
-    </row>
-    <row r="137" spans="1:23">
+      <c r="X136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:24">
       <c r="A137">
         <v>6900</v>
       </c>
@@ -10172,8 +10583,11 @@
       <c r="W137">
         <v>10</v>
       </c>
-    </row>
-    <row r="138" spans="1:23">
+      <c r="X137">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:24">
       <c r="A138">
         <v>6950</v>
       </c>
@@ -10243,8 +10657,11 @@
       <c r="W138">
         <v>10</v>
       </c>
-    </row>
-    <row r="139" spans="1:23">
+      <c r="X138">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24">
       <c r="A139">
         <v>7000</v>
       </c>
@@ -10314,8 +10731,11 @@
       <c r="W139">
         <v>10</v>
       </c>
-    </row>
-    <row r="140" spans="1:23">
+      <c r="X139">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:24">
       <c r="A140">
         <v>7050</v>
       </c>
@@ -10385,8 +10805,11 @@
       <c r="W140">
         <v>10</v>
       </c>
-    </row>
-    <row r="141" spans="1:23">
+      <c r="X140">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24">
       <c r="A141">
         <v>7100</v>
       </c>
@@ -10456,8 +10879,11 @@
       <c r="W141">
         <v>10</v>
       </c>
-    </row>
-    <row r="142" spans="1:23">
+      <c r="X141">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24">
       <c r="A142">
         <v>7150</v>
       </c>
@@ -10527,8 +10953,11 @@
       <c r="W142">
         <v>10</v>
       </c>
-    </row>
-    <row r="143" spans="1:23">
+      <c r="X142">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:24">
       <c r="A143">
         <v>7200</v>
       </c>
@@ -10598,8 +11027,11 @@
       <c r="W143">
         <v>11</v>
       </c>
-    </row>
-    <row r="144" spans="1:23">
+      <c r="X143">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:24">
       <c r="A144">
         <v>7250</v>
       </c>
@@ -10669,8 +11101,11 @@
       <c r="W144">
         <v>11</v>
       </c>
-    </row>
-    <row r="145" spans="1:23">
+      <c r="X144">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:24">
       <c r="A145">
         <v>7300</v>
       </c>
@@ -10740,8 +11175,11 @@
       <c r="W145">
         <v>11</v>
       </c>
-    </row>
-    <row r="146" spans="1:23">
+      <c r="X145">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24">
       <c r="A146">
         <v>7350</v>
       </c>
@@ -10811,8 +11249,11 @@
       <c r="W146">
         <v>11</v>
       </c>
-    </row>
-    <row r="147" spans="1:23">
+      <c r="X146">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24">
       <c r="A147">
         <v>7400</v>
       </c>
@@ -10882,8 +11323,11 @@
       <c r="W147">
         <v>11</v>
       </c>
-    </row>
-    <row r="148" spans="1:23">
+      <c r="X147">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24">
       <c r="A148">
         <v>7450</v>
       </c>
@@ -10953,8 +11397,11 @@
       <c r="W148">
         <v>11</v>
       </c>
-    </row>
-    <row r="149" spans="1:23">
+      <c r="X148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24">
       <c r="A149">
         <v>7500</v>
       </c>
@@ -11024,8 +11471,11 @@
       <c r="W149">
         <v>11</v>
       </c>
-    </row>
-    <row r="150" spans="1:23">
+      <c r="X149">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24">
       <c r="A150">
         <v>7550</v>
       </c>
@@ -11095,8 +11545,11 @@
       <c r="W150">
         <v>11</v>
       </c>
-    </row>
-    <row r="151" spans="1:23">
+      <c r="X150">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24">
       <c r="A151">
         <v>7600</v>
       </c>
@@ -11166,8 +11619,11 @@
       <c r="W151">
         <v>11</v>
       </c>
-    </row>
-    <row r="152" spans="1:23">
+      <c r="X151">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24">
       <c r="A152">
         <v>7650</v>
       </c>
@@ -11237,8 +11693,11 @@
       <c r="W152">
         <v>12</v>
       </c>
-    </row>
-    <row r="153" spans="1:23">
+      <c r="X152">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:24">
       <c r="A153">
         <v>7700</v>
       </c>
@@ -11308,8 +11767,11 @@
       <c r="W153">
         <v>12</v>
       </c>
-    </row>
-    <row r="154" spans="1:23">
+      <c r="X153">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:24">
       <c r="A154">
         <v>7750</v>
       </c>
@@ -11379,8 +11841,11 @@
       <c r="W154">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" spans="1:23">
+      <c r="X154">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:24">
       <c r="A155">
         <v>7800</v>
       </c>
@@ -11450,8 +11915,11 @@
       <c r="W155">
         <v>12</v>
       </c>
-    </row>
-    <row r="156" spans="1:23">
+      <c r="X155">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:24">
       <c r="A156">
         <v>7850</v>
       </c>
@@ -11521,8 +11989,11 @@
       <c r="W156">
         <v>12</v>
       </c>
-    </row>
-    <row r="157" spans="1:23">
+      <c r="X156">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="157" spans="1:24">
       <c r="A157">
         <v>7900</v>
       </c>
@@ -11592,8 +12063,11 @@
       <c r="W157">
         <v>12</v>
       </c>
-    </row>
-    <row r="158" spans="1:23">
+      <c r="X157">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:24">
       <c r="A158">
         <v>7950</v>
       </c>
@@ -11663,8 +12137,11 @@
       <c r="W158">
         <v>12</v>
       </c>
-    </row>
-    <row r="159" spans="1:23">
+      <c r="X158">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" spans="1:24">
       <c r="A159">
         <v>8000</v>
       </c>
@@ -11734,8 +12211,11 @@
       <c r="W159">
         <v>12</v>
       </c>
-    </row>
-    <row r="160" spans="1:23">
+      <c r="X159">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" spans="1:24">
       <c r="A160">
         <v>8050.000000000001</v>
       </c>
@@ -11805,8 +12285,11 @@
       <c r="W160">
         <v>12</v>
       </c>
-    </row>
-    <row r="161" spans="1:23">
+      <c r="X160">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:24">
       <c r="A161">
         <v>8100</v>
       </c>
@@ -11876,8 +12359,11 @@
       <c r="W161">
         <v>12</v>
       </c>
-    </row>
-    <row r="162" spans="1:23">
+      <c r="X161">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:24">
       <c r="A162">
         <v>8150</v>
       </c>
@@ -11947,8 +12433,11 @@
       <c r="W162">
         <v>12</v>
       </c>
-    </row>
-    <row r="163" spans="1:23">
+      <c r="X162">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" spans="1:24">
       <c r="A163">
         <v>8200</v>
       </c>
@@ -12018,8 +12507,11 @@
       <c r="W163">
         <v>12</v>
       </c>
-    </row>
-    <row r="164" spans="1:23">
+      <c r="X163">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:24">
       <c r="A164">
         <v>8250</v>
       </c>
@@ -12089,8 +12581,11 @@
       <c r="W164">
         <v>12</v>
       </c>
-    </row>
-    <row r="165" spans="1:23">
+      <c r="X164">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:24">
       <c r="A165">
         <v>8300</v>
       </c>
@@ -12160,8 +12655,11 @@
       <c r="W165">
         <v>12</v>
       </c>
-    </row>
-    <row r="166" spans="1:23">
+      <c r="X165">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:24">
       <c r="A166">
         <v>8350</v>
       </c>
@@ -12231,8 +12729,11 @@
       <c r="W166">
         <v>12</v>
       </c>
-    </row>
-    <row r="167" spans="1:23">
+      <c r="X166">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:24">
       <c r="A167">
         <v>8400</v>
       </c>
@@ -12302,8 +12803,11 @@
       <c r="W167">
         <v>12</v>
       </c>
-    </row>
-    <row r="168" spans="1:23">
+      <c r="X167">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="1:24">
       <c r="A168">
         <v>8450</v>
       </c>
@@ -12373,8 +12877,11 @@
       <c r="W168">
         <v>12</v>
       </c>
-    </row>
-    <row r="169" spans="1:23">
+      <c r="X168">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:24">
       <c r="A169">
         <v>8500</v>
       </c>
@@ -12444,8 +12951,11 @@
       <c r="W169">
         <v>12</v>
       </c>
-    </row>
-    <row r="170" spans="1:23">
+      <c r="X169">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:24">
       <c r="A170">
         <v>8550</v>
       </c>
@@ -12515,8 +13025,11 @@
       <c r="W170">
         <v>12</v>
       </c>
-    </row>
-    <row r="171" spans="1:23">
+      <c r="X170">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="1:24">
       <c r="A171">
         <v>8600</v>
       </c>
@@ -12586,8 +13099,11 @@
       <c r="W171">
         <v>12</v>
       </c>
-    </row>
-    <row r="172" spans="1:23">
+      <c r="X171">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="172" spans="1:24">
       <c r="A172">
         <v>8650</v>
       </c>
@@ -12657,8 +13173,11 @@
       <c r="W172">
         <v>12</v>
       </c>
-    </row>
-    <row r="173" spans="1:23">
+      <c r="X172">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:24">
       <c r="A173">
         <v>8700</v>
       </c>
@@ -12728,8 +13247,11 @@
       <c r="W173">
         <v>12</v>
       </c>
-    </row>
-    <row r="174" spans="1:23">
+      <c r="X173">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:24">
       <c r="A174">
         <v>8750</v>
       </c>
@@ -12799,8 +13321,11 @@
       <c r="W174">
         <v>14</v>
       </c>
-    </row>
-    <row r="175" spans="1:23">
+      <c r="X174">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:24">
       <c r="A175">
         <v>8800</v>
       </c>
@@ -12870,8 +13395,11 @@
       <c r="W175">
         <v>14</v>
       </c>
-    </row>
-    <row r="176" spans="1:23">
+      <c r="X175">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:24">
       <c r="A176">
         <v>8850</v>
       </c>
@@ -12941,8 +13469,11 @@
       <c r="W176">
         <v>14</v>
       </c>
-    </row>
-    <row r="177" spans="1:23">
+      <c r="X176">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="177" spans="1:24">
       <c r="A177">
         <v>8900</v>
       </c>
@@ -13012,8 +13543,11 @@
       <c r="W177">
         <v>14</v>
       </c>
-    </row>
-    <row r="178" spans="1:23">
+      <c r="X177">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:24">
       <c r="A178">
         <v>8950</v>
       </c>
@@ -13083,8 +13617,11 @@
       <c r="W178">
         <v>14</v>
       </c>
-    </row>
-    <row r="179" spans="1:23">
+      <c r="X178">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:24">
       <c r="A179">
         <v>9000</v>
       </c>
@@ -13154,8 +13691,11 @@
       <c r="W179">
         <v>14</v>
       </c>
-    </row>
-    <row r="180" spans="1:23">
+      <c r="X179">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:24">
       <c r="A180">
         <v>9050</v>
       </c>
@@ -13225,8 +13765,11 @@
       <c r="W180">
         <v>14</v>
       </c>
-    </row>
-    <row r="181" spans="1:23">
+      <c r="X180">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181" spans="1:24">
       <c r="A181">
         <v>9100</v>
       </c>
@@ -13296,8 +13839,11 @@
       <c r="W181">
         <v>14</v>
       </c>
-    </row>
-    <row r="182" spans="1:23">
+      <c r="X181">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="182" spans="1:24">
       <c r="A182">
         <v>9150</v>
       </c>
@@ -13367,8 +13913,11 @@
       <c r="W182">
         <v>14</v>
       </c>
-    </row>
-    <row r="183" spans="1:23">
+      <c r="X182">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="183" spans="1:24">
       <c r="A183">
         <v>9200</v>
       </c>
@@ -13438,8 +13987,11 @@
       <c r="W183">
         <v>14</v>
       </c>
-    </row>
-    <row r="184" spans="1:23">
+      <c r="X183">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24">
       <c r="A184">
         <v>9250</v>
       </c>
@@ -13509,8 +14061,11 @@
       <c r="W184">
         <v>14</v>
       </c>
-    </row>
-    <row r="185" spans="1:23">
+      <c r="X184">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24">
       <c r="A185">
         <v>9300</v>
       </c>
@@ -13580,8 +14135,11 @@
       <c r="W185">
         <v>14</v>
       </c>
-    </row>
-    <row r="186" spans="1:23">
+      <c r="X185">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186" spans="1:24">
       <c r="A186">
         <v>9350</v>
       </c>
@@ -13651,8 +14209,11 @@
       <c r="W186">
         <v>14</v>
       </c>
-    </row>
-    <row r="187" spans="1:23">
+      <c r="X186">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24">
       <c r="A187">
         <v>9400</v>
       </c>
@@ -13722,8 +14283,11 @@
       <c r="W187">
         <v>14</v>
       </c>
-    </row>
-    <row r="188" spans="1:23">
+      <c r="X187">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24">
       <c r="A188">
         <v>9450</v>
       </c>
@@ -13793,8 +14357,11 @@
       <c r="W188">
         <v>14</v>
       </c>
-    </row>
-    <row r="189" spans="1:23">
+      <c r="X188">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24">
       <c r="A189">
         <v>9500</v>
       </c>
@@ -13864,8 +14431,11 @@
       <c r="W189">
         <v>14</v>
       </c>
-    </row>
-    <row r="190" spans="1:23">
+      <c r="X189">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24">
       <c r="A190">
         <v>9559.860000000001</v>
       </c>
@@ -13935,8 +14505,11 @@
       <c r="W190">
         <v>15</v>
       </c>
-    </row>
-    <row r="191" spans="1:23">
+      <c r="X190">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24">
       <c r="A191">
         <v>9600</v>
       </c>
@@ -14006,8 +14579,11 @@
       <c r="W191">
         <v>15</v>
       </c>
-    </row>
-    <row r="192" spans="1:23">
+      <c r="X191">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="192" spans="1:24">
       <c r="A192">
         <v>9650</v>
       </c>
@@ -14077,8 +14653,11 @@
       <c r="W192">
         <v>15</v>
       </c>
-    </row>
-    <row r="193" spans="1:23">
+      <c r="X192">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="193" spans="1:24">
       <c r="A193">
         <v>9700</v>
       </c>
@@ -14148,8 +14727,11 @@
       <c r="W193">
         <v>15</v>
       </c>
-    </row>
-    <row r="194" spans="1:23">
+      <c r="X193">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="194" spans="1:24">
       <c r="A194">
         <v>9750</v>
       </c>
@@ -14219,8 +14801,11 @@
       <c r="W194">
         <v>15</v>
       </c>
-    </row>
-    <row r="195" spans="1:23">
+      <c r="X194">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:24">
       <c r="A195">
         <v>9784.24</v>
       </c>
@@ -14290,8 +14875,11 @@
       <c r="W195">
         <v>16</v>
       </c>
-    </row>
-    <row r="196" spans="1:23">
+      <c r="X195">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="1:24">
       <c r="A196">
         <v>9834</v>
       </c>
@@ -14360,6 +14948,9 @@
       </c>
       <c r="W196">
         <v>16</v>
+      </c>
+      <c r="X196">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>